<commit_message>
an updated commit message*
</commit_message>
<xml_diff>
--- a/frais_malaoui_taoufik.xlsx
+++ b/frais_malaoui_taoufik.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="59">
   <si>
     <t>prix</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>ffff</t>
+  </si>
+  <si>
+    <t>sss</t>
   </si>
 </sst>
 </file>
@@ -1379,7 +1382,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,19 +1655,22 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
         <v>56</v>
+      </c>
+      <c r="I21" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>